<commit_message>
Added an I2CTestHarness project to re-implement from the bottom up.
</commit_message>
<xml_diff>
--- a/RTC/Docs/Bit Manipulations.xlsx
+++ b/RTC/Docs/Bit Manipulations.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\Visual Studio 2015\Projects\CSpectPlugins\RTC\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AA503C-214E-43BB-B748-1AD5A56EB579}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173E2DD1-E60B-45C2-882B-E6399B6DB400}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{6F23A0B2-C9C4-49DF-B0AF-56048C0655D3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Shifting" sheetId="1" r:id="rId1"/>
-    <sheet name="BCD" sheetId="2" r:id="rId2"/>
+    <sheet name="Shift Write" sheetId="1" r:id="rId1"/>
+    <sheet name="Shift Read" sheetId="3" r:id="rId2"/>
+    <sheet name="BCD" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Bit</t>
   </si>
@@ -86,13 +87,19 @@
   </si>
   <si>
     <t>ValHex</t>
+  </si>
+  <si>
+    <t>ValueDec</t>
+  </si>
+  <si>
+    <t>RIghtBit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +111,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -165,6 +180,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +499,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" sqref="A1:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,22 +564,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <f>A2+1</f>
+        <f t="shared" ref="A3:A10" si="0">A2+1</f>
         <v>1</v>
       </c>
       <c r="B3" s="5">
         <v>43</v>
       </c>
       <c r="C3" s="5" t="str">
-        <f t="shared" ref="C3:C10" si="0">HEX2BIN(B3,8)</f>
+        <f t="shared" ref="C3:C10" si="1">HEX2BIN(B3,8)</f>
         <v>01000011</v>
       </c>
       <c r="D3" s="7">
-        <f t="shared" ref="D3:D10" si="1">RIGHT(C3,1) * 1</f>
+        <f t="shared" ref="D3:D10" si="2">RIGHT(C3,1) * 1</f>
         <v>1</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" ref="E3:E9" si="2">_xlfn.BITLSHIFT(D3, 7 - A3)</f>
+        <f t="shared" ref="E3:E9" si="3">_xlfn.BITLSHIFT(D3, 7 - A3)</f>
         <v>64</v>
       </c>
       <c r="F3" s="5">
@@ -571,198 +587,198 @@
         <v>192</v>
       </c>
       <c r="G3" s="5" t="str">
-        <f t="shared" ref="G3:G9" si="3">DEC2HEX(F3, 2)</f>
+        <f t="shared" ref="G3:G9" si="4">DEC2HEX(F3, 2)</f>
         <v>C0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <f>A3+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B4" s="5">
         <v>86</v>
       </c>
       <c r="C4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10000110</v>
       </c>
       <c r="D4" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F4" s="5">
-        <f t="shared" ref="F4:F9" si="4">F3+E4</f>
+        <f t="shared" ref="F4:F9" si="5">F3+E4</f>
         <v>192</v>
       </c>
       <c r="G4" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>C0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <f>A4+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00001101</v>
       </c>
       <c r="D5" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="F5" s="5">
+        <f t="shared" si="5"/>
+        <v>208</v>
+      </c>
+      <c r="G5" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>208</v>
-      </c>
-      <c r="G5" s="5" t="str">
-        <f t="shared" si="3"/>
         <v>D0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <f>A5+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00011010</v>
       </c>
       <c r="D6" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E6" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F6" s="5">
+        <f t="shared" si="5"/>
+        <v>208</v>
+      </c>
+      <c r="G6" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>208</v>
-      </c>
-      <c r="G6" s="5" t="str">
-        <f t="shared" si="3"/>
         <v>D0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <f>A6+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B7" s="5">
         <v>34</v>
       </c>
       <c r="C7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00110100</v>
       </c>
       <c r="D7" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E7" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F7" s="5">
+        <f t="shared" si="5"/>
+        <v>208</v>
+      </c>
+      <c r="G7" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>208</v>
-      </c>
-      <c r="G7" s="5" t="str">
-        <f t="shared" si="3"/>
         <v>D0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <f>A7+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B8" s="5">
         <v>68</v>
       </c>
       <c r="C8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>01101000</v>
       </c>
       <c r="D8" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F8" s="5">
+        <f t="shared" si="5"/>
+        <v>208</v>
+      </c>
+      <c r="G8" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>208</v>
-      </c>
-      <c r="G8" s="5" t="str">
-        <f t="shared" si="3"/>
         <v>D0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <f>A8+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11010000</v>
       </c>
       <c r="D9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F9" s="5">
+        <f t="shared" si="5"/>
+        <v>208</v>
+      </c>
+      <c r="G9" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>208</v>
-      </c>
-      <c r="G9" s="5" t="str">
-        <f t="shared" si="3"/>
         <v>D0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <f>A9+1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000001</v>
       </c>
       <c r="D10" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -773,11 +789,235 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B16F3B2-62B5-44E4-9A79-E57D5417D558}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="9" t="str">
+        <f>DEC2BIN(B2, 8)</f>
+        <v>01011010</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5">
+        <v>90</v>
+      </c>
+      <c r="C2" s="5" t="str">
+        <f>HEX2BIN(B2,8)</f>
+        <v>10010000</v>
+      </c>
+      <c r="D2" s="5">
+        <f>_xlfn.BITRSHIFT(B2, 7 - A2)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <f>_xlfn.BITAND(D2, 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <f t="shared" ref="A3:A10" si="0">A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
+        <v>90</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <f t="shared" ref="C3:C10" si="1">HEX2BIN(B3,8)</f>
+        <v>10010000</v>
+      </c>
+      <c r="D3" s="5">
+        <f t="shared" ref="D3:D9" si="2">_xlfn.BITRSHIFT(B3, 7 - A3)</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E9" si="3">_xlfn.BITAND(D3, 1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B4" s="5">
+        <v>90</v>
+      </c>
+      <c r="C4" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>10010000</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="5">
+        <v>90</v>
+      </c>
+      <c r="C5" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>10010000</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="5">
+        <v>90</v>
+      </c>
+      <c r="C6" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>10010000</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="5">
+        <v>90</v>
+      </c>
+      <c r="C7" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>10010000</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="5">
+        <v>90</v>
+      </c>
+      <c r="C8" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>10010000</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="5">
+        <v>90</v>
+      </c>
+      <c r="C9" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>10010000</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="5">
+        <v>90</v>
+      </c>
+      <c r="C10" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>10010000</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92124506-C410-43E2-B1C3-AF5F21BD14AE}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Setting date/time (by writing to registers 0..6 and stopping) now calculates an offset which is applied to current PC time when reading registers. Fixed a bug with stop command states.
</commit_message>
<xml_diff>
--- a/RTC/Docs/Bit Manipulations.xlsx
+++ b/RTC/Docs/Bit Manipulations.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\Visual Studio 2015\Projects\CSpectPlugins\RTC\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173E2DD1-E60B-45C2-882B-E6399B6DB400}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DB6130-0D88-4E2F-B8E5-99D822B255DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{6F23A0B2-C9C4-49DF-B0AF-56048C0655D3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{6F23A0B2-C9C4-49DF-B0AF-56048C0655D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Shift Write" sheetId="1" r:id="rId1"/>
     <sheet name="Shift Read" sheetId="3" r:id="rId2"/>
     <sheet name="BCD" sheetId="2" r:id="rId3"/>
+    <sheet name="Reg" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Bit</t>
   </si>
@@ -93,6 +94,12 @@
   </si>
   <si>
     <t>RIghtBit</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>Val</t>
   </si>
 </sst>
 </file>
@@ -792,7 +799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B16F3B2-62B5-44E4-9A79-E57D5417D558}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10:C10"/>
     </sheetView>
@@ -1129,4 +1136,50 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11222F75-7280-4A75-8949-1A47DAE732AA}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3">
+        <f>_xlfn.BITAND(B2,15)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
+        <v>166</v>
+      </c>
+      <c r="C3" s="3" t="str">
+        <f>DEC2BIN(B3, 8)</f>
+        <v>10100110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
 </file>
</xml_diff>